<commit_message>
update talk and teaching section
</commit_message>
<xml_diff>
--- a/cv/cv.xlsx
+++ b/cv/cv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristian/Dropbox/Documents/cv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristian/Dropbox/git-repos/cris_blog/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B13BCE-10AC-FD4A-A2F5-271EA35A1EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1547FADF-3A5E-8647-B66B-423B13F6CD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="680" windowWidth="27660" windowHeight="16460" activeTab="4" xr2:uid="{DA4E0661-7526-1B46-BFDD-FC359AB20183}"/>
   </bookViews>
@@ -17,8 +17,9 @@
     <sheet name="education" sheetId="1" r:id="rId2"/>
     <sheet name="research_experience" sheetId="8" r:id="rId3"/>
     <sheet name="teaching" sheetId="3" r:id="rId4"/>
-    <sheet name="talks" sheetId="6" r:id="rId5"/>
-    <sheet name="grants" sheetId="4" r:id="rId6"/>
+    <sheet name="supervision" sheetId="9" r:id="rId5"/>
+    <sheet name="talks" sheetId="6" r:id="rId6"/>
+    <sheet name="grants" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
   <si>
     <t>degree</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Supervisor of a Master's thesis</t>
   </si>
   <si>
-    <t>Lecturer of Introduction to Meta-analysis</t>
-  </si>
-  <si>
     <t>event</t>
   </si>
   <si>
@@ -261,9 +259,6 @@
     <t>Conducted a workshop on the use of the 1080 Sprint resistance device to measure power–velocity profiles and estimate drag in swimmers.</t>
   </si>
   <si>
-    <t>Co-supervised four students in creating a tool to explore the feasability of extracting data from published studies</t>
-  </si>
-  <si>
     <t>Co-supervised four students creating a tool to extract sample sizes from published studies</t>
   </si>
   <si>
@@ -315,13 +310,31 @@
     <t>Discussed whether research published in sports and exercise science journals complies with the Declaration of Helsinki, particularly in light of recent projects highlighting replication and reproducibility issues that contribute to research waste. The slides are available here: https://osf.io/bzp4s/files</t>
   </si>
   <si>
-    <t xml:space="preserve"> Teaching multiple regression, power analysis, and equivalence testing.  Teaching materials can be found at </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taught Introduction to Meta-analysis as part of the Metascience course. Teaching materials can be found at </t>
-  </si>
-  <si>
     <t>2024-Presentation</t>
+  </si>
+  <si>
+    <t>Dutch Research Council</t>
+  </si>
+  <si>
+    <t>Replication studies</t>
+  </si>
+  <si>
+    <t>Assess the reproducibility of power analyses in large-scale replication projects. See project details at https://doi.org/10.61686/FSWVF35053</t>
+  </si>
+  <si>
+    <t>Lecturer of Metascience</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teaching multiple regression, power analysis, and equivalence testing.  Teaching materials can be found at https://cristianmesquida.github.io/multiple_regression/</t>
+  </si>
+  <si>
+    <t>Teaching Introduction to Meta-analysis as part of the Metascience course. Teaching materials can be found at https://github.com/cristianmesquida/introduction_to_meta-analysis</t>
+  </si>
+  <si>
+    <t>Supervisor of Mester End Project</t>
+  </si>
+  <si>
+    <t>Co-supervised a student who used automated search extraction (Metacheck) to extract hypotheses from academic articles and attempted to classify them using large language models</t>
   </si>
 </sst>
 </file>
@@ -776,7 +789,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -784,7 +797,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -793,7 +806,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +853,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -925,7 +938,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -942,53 +955,53 @@
     </row>
     <row r="2" spans="1:5" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="10">
         <v>2018</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="10" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="10">
         <v>2017</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -998,17 +1011,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531F101D-2B48-9F46-A53F-FA67ACC31D52}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.33203125" style="7" customWidth="1"/>
     <col min="2" max="3" width="31" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="7"/>
+    <col min="4" max="4" width="17.6640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="67.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1029,165 +1042,97 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2025</v>
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>35</v>
+      <c r="A4" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>93</v>
+        <v>47</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2024</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>88</v>
+      <c r="A5" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3">
         <v>2024</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2024</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2023</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="3">
-        <v>2023</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2021</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
+    <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1195,10 +1140,117 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0F6311-6111-6149-8D98-BE8A9A017CC2}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2025</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2025</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2024</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2023</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A465BE91-A970-8F4B-854C-C3F13E65FCA4}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1213,7 +1265,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1230,58 +1282,58 @@
     </row>
     <row r="2" spans="1:5" s="13" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5">
         <v>2025</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="5">
         <v>2025</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5">
         <v>2025</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="5">
         <v>2025</v>
@@ -1290,32 +1342,32 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="5">
         <v>2024</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5">
         <v>2024</v>
@@ -1324,44 +1376,44 @@
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="5">
         <v>2019</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1372,12 +1424,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C77CB8-88D5-B640-9A7F-46D72B331807}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1402,17 +1454,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2026</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="3">
         <v>2024</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>